<commit_message>
Note added and DB fixed
</commit_message>
<xml_diff>
--- a/Data/Hit_Location_Source.xlsx
+++ b/Data/Hit_Location_Source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Stat_blocks\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FF2D9E-0901-4F50-8D11-5F09C9E228C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900A3C55-CBFA-4F62-8447-B1CB9120CBE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="15345" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="15345" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Humanoid" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,15 @@
     <sheet name="Beetle" sheetId="5" r:id="rId5"/>
     <sheet name="Wyvern" sheetId="6" r:id="rId6"/>
     <sheet name="Krashtkid" sheetId="7" r:id="rId7"/>
-    <sheet name="Harpy" sheetId="8" r:id="rId10"/>
+    <sheet name="Harpy" sheetId="8" r:id="rId8"/>
+    <sheet name="Lesser Hydra" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Location</t>
   </si>
@@ -440,6 +441,12 @@
   </si>
   <si>
     <t>18-20</t>
+  </si>
+  <si>
+    <t>Heads</t>
+  </si>
+  <si>
+    <t>03-20</t>
   </si>
 </sst>
 </file>
@@ -1725,7 +1732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -1856,8 +1863,134 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="0">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="0">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="0">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="0">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="0">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="0">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="0">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1879,100 +2012,30 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>78</v>
       </c>
       <c r="C2" s="0">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D2" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C3" s="0">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D3" s="0">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="0">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="0">
-        <v>1</v>
-      </c>
-      <c r="D5" s="0">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="0">
-        <v>1</v>
-      </c>
-      <c r="D6" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="0">
-        <v>1</v>
-      </c>
-      <c r="D7" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="0">
-        <v>1</v>
-      </c>
-      <c r="D8" s="0">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
skills, languages and others all cleared up
</commit_message>
<xml_diff>
--- a/Data/Hit_Location_Source.xlsx
+++ b/Data/Hit_Location_Source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Stat_blocks\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900A3C55-CBFA-4F62-8447-B1CB9120CBE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E1ACD3-5449-459B-A1F8-96FF7A60F90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="15345" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="30090" windowHeight="15345" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Humanoid" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="Scorpionman" sheetId="3" r:id="rId4"/>
     <sheet name="Beetle" sheetId="5" r:id="rId5"/>
     <sheet name="Wyvern" sheetId="6" r:id="rId6"/>
-    <sheet name="Krashtkid" sheetId="7" r:id="rId7"/>
-    <sheet name="Harpy" sheetId="8" r:id="rId8"/>
-    <sheet name="Lesser Hydra" sheetId="9" r:id="rId11"/>
+    <sheet name="Harpy" sheetId="8" r:id="rId7"/>
+    <sheet name="Lesser Hydra" sheetId="9" r:id="rId8"/>
+    <sheet name="Krashtkid" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
@@ -401,6 +401,33 @@
     <t>15-16</t>
   </si>
   <si>
+    <t>01-02</t>
+  </si>
+  <si>
+    <t>03-04</t>
+  </si>
+  <si>
+    <t>08-09</t>
+  </si>
+  <si>
+    <t>10-13</t>
+  </si>
+  <si>
+    <t>14-17</t>
+  </si>
+  <si>
+    <t>18-20</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Heads</t>
+  </si>
+  <si>
+    <t>03-20</t>
+  </si>
+  <si>
     <t>01-03</t>
   </si>
   <si>
@@ -419,34 +446,7 @@
     <t>16-18</t>
   </si>
   <si>
-    <t>Body</t>
-  </si>
-  <si>
     <t>19-20</t>
-  </si>
-  <si>
-    <t>01-02</t>
-  </si>
-  <si>
-    <t>03-04</t>
-  </si>
-  <si>
-    <t>08-09</t>
-  </si>
-  <si>
-    <t>10-13</t>
-  </si>
-  <si>
-    <t>14-17</t>
-  </si>
-  <si>
-    <t>18-20</t>
-  </si>
-  <si>
-    <t>Heads</t>
-  </si>
-  <si>
-    <t>03-20</t>
   </si>
 </sst>
 </file>
@@ -1072,6 +1072,131 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="0">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="0">
+        <v>3</v>
+      </c>
+      <c r="D3" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="0">
+        <v>3</v>
+      </c>
+      <c r="D4" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="0">
+        <v>3</v>
+      </c>
+      <c r="D5" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="0">
+        <v>3</v>
+      </c>
+      <c r="D6" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="0">
+        <v>3</v>
+      </c>
+      <c r="D7" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="0">
+        <v>7</v>
+      </c>
+      <c r="D8" s="0">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
@@ -1729,20 +1854,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" bestFit="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" bestFit="1" width="5.83203125" customWidth="1"/>
-    <col min="3" max="3" bestFit="1" width="6.83203125" customWidth="1"/>
-    <col min="4" max="4" bestFit="1" width="3.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
@@ -1760,13 +1877,13 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" s="0">
         <v>4</v>
@@ -1774,13 +1891,13 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>71</v>
       </c>
       <c r="C3" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" s="0">
         <v>4</v>
@@ -1788,72 +1905,72 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C4" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C8" s="0">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D8" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1863,8 +1980,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1886,159 +2003,34 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C2" s="0">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D2" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="0">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D3" s="0">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="0">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="0">
-        <v>1</v>
-      </c>
-      <c r="D5" s="0">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="0">
-        <v>1</v>
-      </c>
-      <c r="D6" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="0">
-        <v>1</v>
-      </c>
-      <c r="D7" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="0">
-        <v>1</v>
-      </c>
-      <c r="D8" s="0">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="0">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="0">
-        <v>6</v>
-      </c>
-      <c r="D3" s="0">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>